<commit_message>
Nielsen data processing + taxonomy creation
</commit_message>
<xml_diff>
--- a/taxonomy_test.xlsx
+++ b/taxonomy_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abeurope-my.sharepoint.com/personal/mattias_mutso_externi_cz/Documents/Documents/AsahiUK_MMM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{CE1BE4AF-01C3-4C0D-AD71-7FE9AD960272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D22F684-36FE-44DE-8F2C-2A4808D3FB91}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{CE1BE4AF-01C3-4C0D-AD71-7FE9AD960272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10C50C17-9689-452A-9031-B0EDFB403543}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{76ACBFB2-FDB9-4F29-83E0-3CEBBBD05A87}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="68">
   <si>
     <t>variable_name</t>
   </si>
@@ -222,6 +222,24 @@
   </si>
   <si>
     <t>spend</t>
+  </si>
+  <si>
+    <t>mod_vol_pna00_impulse_glass_330ml_1_12pack</t>
+  </si>
+  <si>
+    <t>mod_vol_</t>
+  </si>
+  <si>
+    <t>PNA00_IMPULSE_GLASS_330ML_1-12PACK</t>
+  </si>
+  <si>
+    <t>pna00_impulse_glass_330ml_1_12pack</t>
+  </si>
+  <si>
+    <t>mod_dist_pna00_impulse_glass_330ml_1_12pack</t>
+  </si>
+  <si>
+    <t>mod_dist_</t>
   </si>
 </sst>
 </file>
@@ -584,16 +602,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{538DC1F5-E4A4-461E-8C87-E865C98C4EFC}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="30.1796875" customWidth="1"/>
+    <col min="1" max="1" width="43.36328125" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
     <col min="3" max="3" width="12.81640625" customWidth="1"/>
-    <col min="4" max="4" width="25.54296875" customWidth="1"/>
-    <col min="5" max="5" width="20.90625" customWidth="1"/>
+    <col min="4" max="4" width="29.90625" customWidth="1"/>
+    <col min="5" max="5" width="32.1796875" customWidth="1"/>
     <col min="6" max="7" width="19.26953125" customWidth="1"/>
     <col min="8" max="8" width="14.6328125" customWidth="1"/>
     <col min="9" max="9" width="11.6328125" customWidth="1"/>
@@ -629,51 +648,40 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" t="str">
-        <f>C2&amp;E2&amp;G2</f>
-        <v>dep_peroni_btl_12p_330_vol</v>
+      <c r="A2" t="s">
+        <v>62</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="H2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="str">
-        <f t="shared" ref="A3:A16" si="0">C3&amp;E3&amp;G3</f>
-        <v>dep_peroni_btl_sin_620_vol</v>
+      <c r="A3" t="s">
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="G3" t="s">
         <v>33</v>
@@ -684,7 +692,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A3:A16" si="0">C4&amp;E4&amp;G4</f>
         <v>dep_peroni_can_10p_330_vol</v>
       </c>
       <c r="B4" t="s">

</xml_diff>